<commit_message>
Added graph and fixed mean for download and upload
</commit_message>
<xml_diff>
--- a/datasheet.xlsx
+++ b/datasheet.xlsx
@@ -6,6 +6,7 @@
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Hanson" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="Old Main" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="DIFF" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$C$12:$C$44</definedName>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="74">
   <si>
     <t>Website to run test (local): http://speedtest.augustana.edu/</t>
   </si>
@@ -229,6 +230,15 @@
   <si>
     <t xml:space="preserve">Samsung </t>
   </si>
+  <si>
+    <t>DIFF Download Speed</t>
+  </si>
+  <si>
+    <t>DIFF Upload Speed</t>
+  </si>
+  <si>
+    <t>SAMPLE MEAN</t>
+  </si>
 </sst>
 </file>
 
@@ -420,7 +430,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="120">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -685,24 +695,15 @@
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="11" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="11" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="11" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="8" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="9" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="9" fillId="4" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -712,28 +713,83 @@
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="9" fillId="4" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="10" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="21" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="21" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="11">
     <dxf>
       <font/>
       <fill>
@@ -751,7 +807,139 @@
       </fill>
       <border/>
     </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF4DD0E1"/>
+          <bgColor rgb="FF4DD0E1"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE0F7FA"/>
+          <bgColor rgb="FFE0F7FA"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEF8E3"/>
+          <bgColor rgb="FFFEF8E3"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9DAF8"/>
+          <bgColor rgb="FFC9DAF8"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE8F0FE"/>
+          <bgColor rgb="FFE8F0FE"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE7F9EF"/>
+          <bgColor rgb="FFE7F9EF"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEEF7E3"/>
+          <bgColor rgb="FFEEF7E3"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
   </dxfs>
+  <tableStyles count="8">
+    <tableStyle count="3" pivot="0" name="Hanson-style">
+      <tableStyleElement dxfId="2" type="headerRow"/>
+      <tableStyleElement dxfId="3" type="firstRowStripe"/>
+      <tableStyleElement dxfId="4" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="3" pivot="0" name="Hanson-style 2">
+      <tableStyleElement dxfId="5" type="headerRow"/>
+      <tableStyleElement dxfId="3" type="firstRowStripe"/>
+      <tableStyleElement dxfId="6" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="3" pivot="0" name="Hanson-style 3">
+      <tableStyleElement dxfId="7" type="headerRow"/>
+      <tableStyleElement dxfId="3" type="firstRowStripe"/>
+      <tableStyleElement dxfId="8" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="3" pivot="0" name="Hanson-style 4">
+      <tableStyleElement dxfId="9" type="headerRow"/>
+      <tableStyleElement dxfId="3" type="firstRowStripe"/>
+      <tableStyleElement dxfId="10" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="3" pivot="0" name="Old Main-style">
+      <tableStyleElement dxfId="2" type="headerRow"/>
+      <tableStyleElement dxfId="3" type="firstRowStripe"/>
+      <tableStyleElement dxfId="4" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="3" pivot="0" name="Old Main-style 2">
+      <tableStyleElement dxfId="5" type="headerRow"/>
+      <tableStyleElement dxfId="3" type="firstRowStripe"/>
+      <tableStyleElement dxfId="6" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="3" pivot="0" name="Old Main-style 3">
+      <tableStyleElement dxfId="7" type="headerRow"/>
+      <tableStyleElement dxfId="3" type="firstRowStripe"/>
+      <tableStyleElement dxfId="8" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="3" pivot="0" name="Old Main-style 4">
+      <tableStyleElement dxfId="9" type="headerRow"/>
+      <tableStyleElement dxfId="3" type="firstRowStripe"/>
+      <tableStyleElement dxfId="10" type="secondRowStripe"/>
+    </tableStyle>
+  </tableStyles>
 </styleSheet>
 </file>
 
@@ -840,11 +1028,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="476440151"/>
-        <c:axId val="1238345381"/>
+        <c:axId val="2052167581"/>
+        <c:axId val="143307306"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="476440151"/>
+        <c:axId val="2052167581"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -896,10 +1084,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1238345381"/>
+        <c:crossAx val="143307306"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1238345381"/>
+        <c:axId val="143307306"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -974,7 +1162,262 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="476440151"/>
+        <c:crossAx val="2052167581"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>DIFF Download Speed and DIFF Upload Speed</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>DIFF!$B$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>DIFF!$A$2:$A$17</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>DIFF!$B$2:$B$17</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>DIFF!$C$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>DIFF!$A$2:$A$17</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>DIFF!$C$2:$C$17</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="1002337092"/>
+        <c:axId val="899006034"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1002337092"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t>Date</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="899006034"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="899006034"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1002337092"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1036,6 +1479,210 @@
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="6924675" cy="3533775"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 2" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:J5" displayName="Table_1" id="1">
+  <tableColumns count="10">
+    <tableColumn name="Location" id="1"/>
+    <tableColumn name="Date" id="2"/>
+    <tableColumn name="Expected Time" id="3"/>
+    <tableColumn name="Actual Time" id="4"/>
+    <tableColumn name="Download Speed (Mbps)" id="5"/>
+    <tableColumn name="Upload Speed (Mbps)" id="6"/>
+    <tableColumn name="Ping (milli sec.)" id="7"/>
+    <tableColumn name="Jitter (ms)" id="8"/>
+    <tableColumn name="Device Manufacturer" id="9"/>
+    <tableColumn name="Device Model" id="10"/>
+  </tableColumns>
+  <tableStyleInfo name="Hanson-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A6:J9" displayName="Table_2" id="2">
+  <tableColumns count="10">
+    <tableColumn name="Column1" id="1"/>
+    <tableColumn name="Column2" id="2"/>
+    <tableColumn name="Column3" id="3"/>
+    <tableColumn name="Column4" id="4"/>
+    <tableColumn name="Column5" id="5"/>
+    <tableColumn name="Column6" id="6"/>
+    <tableColumn name="Column7" id="7"/>
+    <tableColumn name="Column8" id="8"/>
+    <tableColumn name="Column9" id="9"/>
+    <tableColumn name="Column10" id="10"/>
+  </tableColumns>
+  <tableStyleInfo name="Hanson-style 2" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
+    </ext>
+  </extLst>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A10:J13" displayName="Table_3" id="3">
+  <tableColumns count="10">
+    <tableColumn name="Column1" id="1"/>
+    <tableColumn name="Column2" id="2"/>
+    <tableColumn name="Column3" id="3"/>
+    <tableColumn name="Column4" id="4"/>
+    <tableColumn name="Column5" id="5"/>
+    <tableColumn name="Column6" id="6"/>
+    <tableColumn name="Column7" id="7"/>
+    <tableColumn name="Column8" id="8"/>
+    <tableColumn name="Column9" id="9"/>
+    <tableColumn name="Column10" id="10"/>
+  </tableColumns>
+  <tableStyleInfo name="Hanson-style 3" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
+    </ext>
+  </extLst>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A14:J17" displayName="Table_4" id="4">
+  <tableColumns count="10">
+    <tableColumn name="Column1" id="1"/>
+    <tableColumn name="Column2" id="2"/>
+    <tableColumn name="Column3" id="3"/>
+    <tableColumn name="Column4" id="4"/>
+    <tableColumn name="Column5" id="5"/>
+    <tableColumn name="Column6" id="6"/>
+    <tableColumn name="Column7" id="7"/>
+    <tableColumn name="Column8" id="8"/>
+    <tableColumn name="Column9" id="9"/>
+    <tableColumn name="Column10" id="10"/>
+  </tableColumns>
+  <tableStyleInfo name="Hanson-style 4" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
+    </ext>
+  </extLst>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:J5" displayName="Table_5" id="5">
+  <tableColumns count="10">
+    <tableColumn name="Location" id="1"/>
+    <tableColumn name="Date" id="2"/>
+    <tableColumn name="Expected Time" id="3"/>
+    <tableColumn name="Actual Time" id="4"/>
+    <tableColumn name="Download Speed (Mbps)" id="5"/>
+    <tableColumn name="Upload Speed (Mbps)" id="6"/>
+    <tableColumn name="Ping (milli sec.)" id="7"/>
+    <tableColumn name="Jitter (ms)" id="8"/>
+    <tableColumn name="Device Manufacturer" id="9"/>
+    <tableColumn name="Device Model" id="10"/>
+  </tableColumns>
+  <tableStyleInfo name="Old Main-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A6:J9" displayName="Table_6" id="6">
+  <tableColumns count="10">
+    <tableColumn name="Column1" id="1"/>
+    <tableColumn name="Column2" id="2"/>
+    <tableColumn name="Column3" id="3"/>
+    <tableColumn name="Column4" id="4"/>
+    <tableColumn name="Column5" id="5"/>
+    <tableColumn name="Column6" id="6"/>
+    <tableColumn name="Column7" id="7"/>
+    <tableColumn name="Column8" id="8"/>
+    <tableColumn name="Column9" id="9"/>
+    <tableColumn name="Column10" id="10"/>
+  </tableColumns>
+  <tableStyleInfo name="Old Main-style 2" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
+    </ext>
+  </extLst>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A10:J13" displayName="Table_7" id="7">
+  <tableColumns count="10">
+    <tableColumn name="Column1" id="1"/>
+    <tableColumn name="Column2" id="2"/>
+    <tableColumn name="Column3" id="3"/>
+    <tableColumn name="Column4" id="4"/>
+    <tableColumn name="Column5" id="5"/>
+    <tableColumn name="Column6" id="6"/>
+    <tableColumn name="Column7" id="7"/>
+    <tableColumn name="Column8" id="8"/>
+    <tableColumn name="Column9" id="9"/>
+    <tableColumn name="Column10" id="10"/>
+  </tableColumns>
+  <tableStyleInfo name="Old Main-style 3" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
+    </ext>
+  </extLst>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A14:J17" displayName="Table_8" id="8">
+  <tableColumns count="10">
+    <tableColumn name="Column1" id="1"/>
+    <tableColumn name="Column2" id="2"/>
+    <tableColumn name="Column3" id="3"/>
+    <tableColumn name="Column4" id="4"/>
+    <tableColumn name="Column5" id="5"/>
+    <tableColumn name="Column6" id="6"/>
+    <tableColumn name="Column7" id="7"/>
+    <tableColumn name="Column8" id="8"/>
+    <tableColumn name="Column9" id="9"/>
+    <tableColumn name="Column10" id="10"/>
+  </tableColumns>
+  <tableStyleInfo name="Old Main-style 4" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
+    </ext>
+  </extLst>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1251,7 +1898,7 @@
     <col customWidth="1" min="14" max="14" width="14.38"/>
     <col customWidth="1" min="15" max="15" width="15.25"/>
     <col customWidth="1" min="16" max="16" width="13.38"/>
-    <col customWidth="1" min="17" max="17" width="35.13"/>
+    <col customWidth="1" min="17" max="17" width="56.13"/>
     <col customWidth="1" min="18" max="18" width="46.88"/>
   </cols>
   <sheetData>
@@ -1457,7 +2104,7 @@
       <c r="AG13" s="9"/>
       <c r="AH13" s="9"/>
     </row>
-    <row r="14" hidden="1">
+    <row r="14">
       <c r="A14" s="16" t="b">
         <v>1</v>
       </c>
@@ -1593,7 +2240,7 @@
       <c r="AG15" s="9"/>
       <c r="AH15" s="9"/>
     </row>
-    <row r="16" hidden="1">
+    <row r="16">
       <c r="A16" s="16" t="b">
         <v>1</v>
       </c>
@@ -1727,7 +2374,7 @@
       <c r="AG17" s="9"/>
       <c r="AH17" s="9"/>
     </row>
-    <row r="18" hidden="1">
+    <row r="18">
       <c r="A18" s="16" t="b">
         <v>1</v>
       </c>
@@ -1863,7 +2510,7 @@
       <c r="AG19" s="9"/>
       <c r="AH19" s="9"/>
     </row>
-    <row r="20" hidden="1">
+    <row r="20">
       <c r="A20" s="31" t="b">
         <v>1</v>
       </c>
@@ -2001,7 +2648,7 @@
       <c r="AG21" s="9"/>
       <c r="AH21" s="9"/>
     </row>
-    <row r="22" hidden="1">
+    <row r="22">
       <c r="A22" s="22" t="b">
         <v>1</v>
       </c>
@@ -2139,7 +2786,7 @@
       <c r="AG23" s="9"/>
       <c r="AH23" s="9"/>
     </row>
-    <row r="24" hidden="1">
+    <row r="24">
       <c r="A24" s="22" t="b">
         <v>1</v>
       </c>
@@ -2281,7 +2928,7 @@
       <c r="AG25" s="9"/>
       <c r="AH25" s="9"/>
     </row>
-    <row r="26" hidden="1">
+    <row r="26">
       <c r="A26" s="22" t="b">
         <v>1</v>
       </c>
@@ -2421,7 +3068,7 @@
       <c r="AG27" s="9"/>
       <c r="AH27" s="9"/>
     </row>
-    <row r="28" hidden="1">
+    <row r="28">
       <c r="A28" s="22" t="b">
         <v>1</v>
       </c>
@@ -2555,7 +3202,7 @@
       <c r="AG29" s="9"/>
       <c r="AH29" s="9"/>
     </row>
-    <row r="30" hidden="1">
+    <row r="30">
       <c r="A30" s="22" t="b">
         <v>1</v>
       </c>
@@ -2691,7 +3338,7 @@
       <c r="AG31" s="9"/>
       <c r="AH31" s="9"/>
     </row>
-    <row r="32" hidden="1">
+    <row r="32">
       <c r="A32" s="22" t="b">
         <v>1</v>
       </c>
@@ -2827,7 +3474,7 @@
       <c r="AG33" s="9"/>
       <c r="AH33" s="9"/>
     </row>
-    <row r="34" hidden="1">
+    <row r="34">
       <c r="A34" s="22" t="b">
         <v>1</v>
       </c>
@@ -2953,7 +3600,7 @@
       <c r="AG35" s="9"/>
       <c r="AH35" s="9"/>
     </row>
-    <row r="36" hidden="1">
+    <row r="36">
       <c r="A36" s="22" t="b">
         <v>1</v>
       </c>
@@ -3019,7 +3666,7 @@
     </row>
     <row r="37">
       <c r="A37" s="73" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B37" s="74" t="s">
         <v>61</v>
@@ -3075,9 +3722,9 @@
       <c r="AG37" s="9"/>
       <c r="AH37" s="9"/>
     </row>
-    <row r="38" hidden="1">
+    <row r="38">
       <c r="A38" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B38" s="15" t="s">
         <v>26</v>
@@ -3109,12 +3756,24 @@
       <c r="K38" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="L38" s="27"/>
-      <c r="M38" s="27"/>
-      <c r="N38" s="27"/>
-      <c r="O38" s="41"/>
-      <c r="P38" s="41"/>
-      <c r="Q38" s="41"/>
+      <c r="L38" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="M38" s="15">
+        <v>2021.0</v>
+      </c>
+      <c r="N38" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="O38" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="P38" s="15">
+        <v>22621.2715</v>
+      </c>
+      <c r="Q38" s="15" t="s">
+        <v>33</v>
+      </c>
       <c r="R38" s="41"/>
       <c r="S38" s="9"/>
       <c r="T38" s="9"/>
@@ -3189,9 +3848,9 @@
       <c r="AG39" s="9"/>
       <c r="AH39" s="9"/>
     </row>
-    <row r="40" hidden="1">
+    <row r="40">
       <c r="A40" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B40" s="15" t="s">
         <v>59</v>
@@ -3220,13 +3879,27 @@
       <c r="J40" s="15">
         <v>28.6</v>
       </c>
-      <c r="K40" s="27"/>
-      <c r="L40" s="27"/>
-      <c r="M40" s="27"/>
-      <c r="N40" s="27"/>
-      <c r="O40" s="41"/>
-      <c r="P40" s="41"/>
-      <c r="Q40" s="41"/>
+      <c r="K40" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="L40" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="M40" s="15">
+        <v>2021.0</v>
+      </c>
+      <c r="N40" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="O40" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="P40" s="15">
+        <v>22621.2715</v>
+      </c>
+      <c r="Q40" s="15" t="s">
+        <v>33</v>
+      </c>
       <c r="R40" s="41"/>
       <c r="S40" s="9"/>
       <c r="T40" s="9"/>
@@ -3247,7 +3920,7 @@
     </row>
     <row r="41">
       <c r="A41" s="80" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B41" s="81" t="s">
         <v>61</v>
@@ -3261,12 +3934,21 @@
       <c r="E41" s="84" t="s">
         <v>44</v>
       </c>
-      <c r="F41" s="89"/>
-      <c r="G41" s="87"/>
-      <c r="H41" s="90"/>
-      <c r="I41" s="87"/>
-      <c r="J41" s="87"/>
-      <c r="K41" s="87"/>
+      <c r="F41" s="89">
+        <v>0.6354166666666666</v>
+      </c>
+      <c r="G41" s="90">
+        <v>2.38</v>
+      </c>
+      <c r="H41" s="90">
+        <v>10.6</v>
+      </c>
+      <c r="I41" s="90">
+        <v>16.0</v>
+      </c>
+      <c r="J41" s="90">
+        <v>412.0</v>
+      </c>
       <c r="L41" s="87"/>
       <c r="M41" s="87"/>
       <c r="N41" s="87"/>
@@ -3291,11 +3973,13 @@
       <c r="AG41" s="9"/>
       <c r="AH41" s="9"/>
     </row>
-    <row r="42" hidden="1">
+    <row r="42">
       <c r="A42" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="B42" s="27"/>
+        <v>1</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>26</v>
+      </c>
       <c r="C42" s="15" t="s">
         <v>35</v>
       </c>
@@ -3305,18 +3989,42 @@
       <c r="E42" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="F42" s="91"/>
-      <c r="G42" s="27"/>
-      <c r="H42" s="92"/>
-      <c r="I42" s="27"/>
-      <c r="J42" s="27"/>
-      <c r="K42" s="27"/>
-      <c r="L42" s="27"/>
-      <c r="M42" s="27"/>
-      <c r="N42" s="27"/>
-      <c r="O42" s="41"/>
-      <c r="P42" s="41"/>
-      <c r="Q42" s="41"/>
+      <c r="F42" s="25">
+        <v>0.125</v>
+      </c>
+      <c r="G42" s="15">
+        <v>106.0</v>
+      </c>
+      <c r="H42" s="26">
+        <v>139.0</v>
+      </c>
+      <c r="I42" s="15">
+        <v>4.1</v>
+      </c>
+      <c r="J42" s="15">
+        <v>10.0</v>
+      </c>
+      <c r="K42" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="L42" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="M42" s="15">
+        <v>2021.0</v>
+      </c>
+      <c r="N42" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="O42" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="P42" s="15">
+        <v>22621.2715</v>
+      </c>
+      <c r="Q42" s="15" t="s">
+        <v>33</v>
+      </c>
       <c r="R42" s="41"/>
       <c r="S42" s="9"/>
       <c r="T42" s="9"/>
@@ -3337,7 +4045,7 @@
     </row>
     <row r="43">
       <c r="A43" s="80" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B43" s="81" t="s">
         <v>61</v>
@@ -3351,11 +4059,21 @@
       <c r="E43" s="84" t="s">
         <v>51</v>
       </c>
-      <c r="F43" s="89"/>
-      <c r="G43" s="87"/>
-      <c r="H43" s="90"/>
-      <c r="I43" s="87"/>
-      <c r="J43" s="87"/>
+      <c r="F43" s="85">
+        <v>0.6881944444444444</v>
+      </c>
+      <c r="G43" s="82">
+        <v>2.93</v>
+      </c>
+      <c r="H43" s="86">
+        <v>13.4</v>
+      </c>
+      <c r="I43" s="82">
+        <v>4.0</v>
+      </c>
+      <c r="J43" s="82">
+        <v>20.6</v>
+      </c>
       <c r="K43" s="87"/>
       <c r="L43" s="87"/>
       <c r="M43" s="87"/>
@@ -3381,32 +4099,58 @@
       <c r="AG43" s="9"/>
       <c r="AH43" s="9"/>
     </row>
-    <row r="44" hidden="1">
-      <c r="A44" s="93" t="b">
-        <v>0</v>
-      </c>
-      <c r="B44" s="94"/>
-      <c r="C44" s="95" t="s">
+    <row r="44">
+      <c r="A44" s="91" t="b">
+        <v>1</v>
+      </c>
+      <c r="B44" s="92" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44" s="92" t="s">
         <v>35</v>
       </c>
-      <c r="D44" s="96">
+      <c r="D44" s="93">
         <v>45266.0</v>
       </c>
-      <c r="E44" s="97" t="s">
+      <c r="E44" s="94" t="s">
         <v>51</v>
       </c>
-      <c r="F44" s="98"/>
-      <c r="G44" s="94"/>
-      <c r="H44" s="99"/>
-      <c r="I44" s="94"/>
-      <c r="J44" s="94"/>
-      <c r="K44" s="94"/>
-      <c r="L44" s="94"/>
-      <c r="M44" s="94"/>
-      <c r="N44" s="94"/>
-      <c r="O44" s="54"/>
-      <c r="P44" s="54"/>
-      <c r="Q44" s="54"/>
+      <c r="F44" s="95">
+        <v>0.19791666666666666</v>
+      </c>
+      <c r="G44" s="92">
+        <v>20.4</v>
+      </c>
+      <c r="H44" s="96">
+        <v>50.2</v>
+      </c>
+      <c r="I44" s="92">
+        <v>5.2</v>
+      </c>
+      <c r="J44" s="92">
+        <v>20.8</v>
+      </c>
+      <c r="K44" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="L44" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="M44" s="15">
+        <v>2021.0</v>
+      </c>
+      <c r="N44" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="O44" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="P44" s="15">
+        <v>22621.2715</v>
+      </c>
+      <c r="Q44" s="15" t="s">
+        <v>33</v>
+      </c>
       <c r="R44" s="54"/>
       <c r="S44" s="9"/>
       <c r="T44" s="9"/>
@@ -6270,13 +7014,7 @@
       <c r="F992" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="$C$12:$C$44">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Old Main"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="$C$12:$C$44"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -6293,270 +7031,560 @@
   <cols>
     <col customWidth="1" min="4" max="4" width="19.38"/>
     <col customWidth="1" min="5" max="5" width="17.25"/>
+    <col customWidth="1" min="10" max="10" width="37.0"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="100" t="s">
+      <c r="C1" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="101" t="s">
+      <c r="D1" s="98" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="100" t="s">
+      <c r="E1" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="100" t="s">
+      <c r="F1" s="97" t="s">
         <v>15</v>
       </c>
+      <c r="G1" s="97" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="97" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="97" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="97" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="102">
+      <c r="A2" s="99" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="100">
         <v>45262.0</v>
       </c>
-      <c r="B2" s="100" t="s">
+      <c r="C2" s="99" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="101">
+      <c r="D2" s="101">
         <v>0.43472222222222223</v>
       </c>
-      <c r="D2" s="100">
+      <c r="E2" s="99">
         <v>240.0</v>
       </c>
-      <c r="E2" s="100">
+      <c r="F2" s="102">
         <v>259.0</v>
       </c>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="103" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="103" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="102">
+      <c r="A3" s="99" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="100">
         <v>45262.0</v>
       </c>
-      <c r="B3" s="100" t="s">
+      <c r="C3" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="101">
+      <c r="D3" s="101">
         <v>0.5604166666666667</v>
       </c>
-      <c r="D3" s="100">
+      <c r="E3" s="99">
         <v>97.8</v>
       </c>
-      <c r="E3" s="100">
+      <c r="F3" s="102">
         <v>97.8</v>
       </c>
+      <c r="G3" s="99">
+        <v>3.0</v>
+      </c>
+      <c r="H3" s="99">
+        <v>0.75</v>
+      </c>
+      <c r="I3" s="99" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" s="99" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="102">
+      <c r="A4" s="99" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="100">
         <v>45262.0</v>
       </c>
-      <c r="B4" s="100" t="s">
+      <c r="C4" s="104" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="101">
+      <c r="D4" s="101">
         <v>0.6256944444444444</v>
       </c>
-      <c r="D4" s="100">
+      <c r="E4" s="99">
         <v>97.3</v>
       </c>
-      <c r="E4" s="100">
+      <c r="F4" s="102">
         <v>90.3</v>
       </c>
+      <c r="G4" s="99">
+        <v>2.6</v>
+      </c>
+      <c r="H4" s="99">
+        <v>0.47</v>
+      </c>
+      <c r="I4" s="99" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="99" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="102">
+      <c r="A5" s="105" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="106">
         <v>45262.0</v>
       </c>
-      <c r="B5" s="100" t="s">
+      <c r="C5" s="107" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="101">
+      <c r="D5" s="101">
         <v>0.6895833333333333</v>
       </c>
-      <c r="D5" s="100">
+      <c r="E5" s="99">
         <v>44.9</v>
       </c>
-      <c r="E5" s="100">
+      <c r="F5" s="102">
         <v>88.0</v>
       </c>
+      <c r="G5" s="99">
+        <v>2.4</v>
+      </c>
+      <c r="H5" s="99">
+        <v>0.77</v>
+      </c>
+      <c r="I5" s="99" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="99" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="102">
+      <c r="A6" s="99" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="100">
         <v>45264.0</v>
       </c>
-      <c r="B6" s="100" t="s">
+      <c r="C6" s="99" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="101">
+      <c r="D6" s="101">
         <v>0.4354166666666667</v>
       </c>
-      <c r="D6" s="100">
+      <c r="E6" s="99">
         <v>28.2</v>
       </c>
-      <c r="E6" s="100">
+      <c r="F6" s="102">
         <v>62.7</v>
       </c>
+      <c r="G6" s="99">
+        <v>8.2</v>
+      </c>
+      <c r="H6" s="99">
+        <v>831.0</v>
+      </c>
+      <c r="I6" s="99" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="99" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="102">
+      <c r="A7" s="99" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="100">
         <v>45264.0</v>
       </c>
-      <c r="B7" s="100" t="s">
+      <c r="C7" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="101">
+      <c r="D7" s="101">
         <v>0.5743055555555555</v>
       </c>
-      <c r="D7" s="100">
+      <c r="E7" s="99">
         <v>35.8</v>
       </c>
-      <c r="E7" s="100">
+      <c r="F7" s="102">
         <v>27.1</v>
       </c>
+      <c r="G7" s="99">
+        <v>5.0</v>
+      </c>
+      <c r="H7" s="99">
+        <v>41.6</v>
+      </c>
+      <c r="I7" s="99" t="s">
+        <v>39</v>
+      </c>
+      <c r="J7" s="99" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="102">
+      <c r="A8" s="99" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="100">
         <v>45264.0</v>
       </c>
-      <c r="B8" s="100" t="s">
+      <c r="C8" s="104" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="101">
+      <c r="D8" s="101">
         <v>0.13541666666666666</v>
       </c>
-      <c r="D8" s="100">
+      <c r="E8" s="99">
         <v>68.5</v>
       </c>
-      <c r="E8" s="100">
+      <c r="F8" s="102">
         <v>26.6</v>
       </c>
+      <c r="G8" s="99">
+        <v>7.6</v>
+      </c>
+      <c r="H8" s="99">
+        <v>25.8</v>
+      </c>
+      <c r="I8" s="99" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="99" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="102">
+      <c r="A9" s="99" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="100">
         <v>45264.0</v>
       </c>
-      <c r="B9" s="100" t="s">
+      <c r="C9" s="104" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="101">
+      <c r="D9" s="101">
         <v>0.6875</v>
       </c>
-      <c r="D9" s="100">
+      <c r="E9" s="99">
         <v>124.0</v>
       </c>
-      <c r="E9" s="100">
+      <c r="F9" s="102">
         <v>56.7</v>
       </c>
+      <c r="G9" s="99">
+        <v>4.5</v>
+      </c>
+      <c r="H9" s="99">
+        <v>22.9</v>
+      </c>
+      <c r="I9" s="99" t="s">
+        <v>39</v>
+      </c>
+      <c r="J9" s="99" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="102">
+      <c r="A10" s="99" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="100">
         <v>45265.0</v>
       </c>
-      <c r="B10" s="100" t="s">
+      <c r="C10" s="99" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="101">
+      <c r="D10" s="101">
         <v>0.4395833333333333</v>
       </c>
-      <c r="D10" s="100">
+      <c r="E10" s="99">
         <v>1.34</v>
       </c>
-      <c r="E10" s="100">
+      <c r="F10" s="102">
         <v>1.69</v>
       </c>
+      <c r="G10" s="99">
+        <v>88.9</v>
+      </c>
+      <c r="H10" s="99">
+        <v>2126.0</v>
+      </c>
+      <c r="I10" s="99" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10" s="99" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="102">
+      <c r="A11" s="99" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="100">
         <v>45265.0</v>
       </c>
-      <c r="B11" s="100" t="s">
+      <c r="C11" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="101">
+      <c r="D11" s="101">
         <v>0.5625</v>
       </c>
-      <c r="D11" s="100">
+      <c r="E11" s="99">
         <v>11.3</v>
       </c>
-      <c r="E11" s="100">
+      <c r="F11" s="102">
         <v>22.3</v>
       </c>
+      <c r="G11" s="99">
+        <v>4.8</v>
+      </c>
+      <c r="H11" s="99">
+        <v>62.2</v>
+      </c>
+      <c r="I11" s="99" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11" s="99" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="102">
+      <c r="A12" s="99" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="100">
         <v>45265.0</v>
       </c>
-      <c r="B12" s="100" t="s">
+      <c r="C12" s="104" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="101">
+      <c r="D12" s="101">
         <v>0.6423611111111112</v>
       </c>
-      <c r="D12" s="100">
+      <c r="E12" s="99">
         <v>140.0</v>
       </c>
-      <c r="E12" s="100">
+      <c r="F12" s="102">
         <v>81.4</v>
       </c>
+      <c r="G12" s="99">
+        <v>2.6</v>
+      </c>
+      <c r="H12" s="99">
+        <v>28.9</v>
+      </c>
+      <c r="I12" s="99" t="s">
+        <v>39</v>
+      </c>
+      <c r="J12" s="108"/>
     </row>
     <row r="13">
-      <c r="A13" s="102">
+      <c r="A13" s="99" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="100">
         <v>45265.0</v>
       </c>
-      <c r="B13" s="100" t="s">
+      <c r="C13" s="104" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="101">
+      <c r="D13" s="101">
         <v>0.6875</v>
       </c>
-      <c r="D13" s="100">
+      <c r="E13" s="99">
         <v>245.0</v>
       </c>
-      <c r="E13" s="100">
+      <c r="F13" s="102">
         <v>189.0</v>
       </c>
+      <c r="G13" s="99">
+        <v>3.6</v>
+      </c>
+      <c r="H13" s="99">
+        <v>0.64</v>
+      </c>
+      <c r="I13" s="99" t="s">
+        <v>39</v>
+      </c>
+      <c r="J13" s="99" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="102">
+      <c r="A14" s="99" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="100">
         <v>45266.0</v>
       </c>
-      <c r="B14" s="100" t="s">
+      <c r="C14" s="99" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="101">
+      <c r="D14" s="109">
         <v>0.43333333333333335</v>
       </c>
-      <c r="D14" s="100">
+      <c r="E14" s="103">
         <v>4.62</v>
       </c>
-      <c r="E14" s="100">
+      <c r="F14" s="110">
         <v>37.3</v>
       </c>
+      <c r="G14" s="103">
+        <v>31.0</v>
+      </c>
+      <c r="H14" s="103">
+        <v>2147.0</v>
+      </c>
+      <c r="I14" s="99" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" s="99" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="102">
+      <c r="A15" s="99" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="100">
         <v>45266.0</v>
       </c>
-      <c r="B15" s="100" t="s">
+      <c r="C15" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="101">
+      <c r="D15" s="101">
         <v>0.06597222222222222</v>
       </c>
-      <c r="D15" s="100">
+      <c r="E15" s="99">
         <v>61.8</v>
       </c>
-      <c r="E15" s="100">
+      <c r="F15" s="102">
         <v>105.0</v>
       </c>
+      <c r="G15" s="99">
+        <v>4.4</v>
+      </c>
+      <c r="H15" s="99">
+        <v>28.6</v>
+      </c>
+      <c r="I15" s="99" t="s">
+        <v>29</v>
+      </c>
+      <c r="J15" s="99" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="99" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="100">
+        <v>45266.0</v>
+      </c>
+      <c r="C16" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="101">
+        <v>0.125</v>
+      </c>
+      <c r="E16" s="99">
+        <v>106.0</v>
+      </c>
+      <c r="F16" s="102">
+        <v>139.0</v>
+      </c>
+      <c r="G16" s="99">
+        <v>4.1</v>
+      </c>
+      <c r="H16" s="99">
+        <v>10.0</v>
+      </c>
+      <c r="I16" s="99" t="s">
+        <v>29</v>
+      </c>
+      <c r="J16" s="99" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="105" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="106">
+        <v>45266.0</v>
+      </c>
+      <c r="C17" s="107" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="111">
+        <v>0.19791666666666666</v>
+      </c>
+      <c r="E17" s="105">
+        <v>20.4</v>
+      </c>
+      <c r="F17" s="112">
+        <v>50.2</v>
+      </c>
+      <c r="G17" s="105">
+        <v>5.2</v>
+      </c>
+      <c r="H17" s="105">
+        <v>20.8</v>
+      </c>
+      <c r="I17" s="99" t="s">
+        <v>29</v>
+      </c>
+      <c r="J17" s="99" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:Z1000">
+  <conditionalFormatting sqref="A1:A1000 B1:J16 K1:Z1000 B18:J1000">
     <cfRule type="notContainsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <drawing r:id="rId1"/>
+  <tableParts count="4">
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -6571,261 +7599,798 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="5" max="5" width="17.25"/>
+    <col customWidth="1" min="10" max="10" width="35.0"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="100" t="s">
+      <c r="C1" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="101" t="s">
+      <c r="D1" s="98" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="100" t="s">
+      <c r="E1" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="100" t="s">
+      <c r="F1" s="97" t="s">
         <v>15</v>
       </c>
+      <c r="G1" s="97" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="97" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="97" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="97" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="102">
+      <c r="A2" s="103" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="113">
         <v>45262.0</v>
       </c>
-      <c r="B2" s="100" t="s">
+      <c r="C2" s="103" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="101">
+      <c r="D2" s="109">
         <v>0.43819444444444444</v>
       </c>
-      <c r="D2" s="100">
+      <c r="E2" s="103">
         <v>312.0</v>
       </c>
-      <c r="E2" s="100">
+      <c r="F2" s="110">
         <v>416.0</v>
       </c>
+      <c r="G2" s="103">
+        <v>2.0</v>
+      </c>
+      <c r="H2" s="103">
+        <v>0.91</v>
+      </c>
+      <c r="I2" s="103" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="103" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="102">
+      <c r="A3" s="99" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="100">
         <v>45262.0</v>
       </c>
-      <c r="B3" s="100" t="s">
+      <c r="C3" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="101">
+      <c r="D3" s="101">
         <v>0.5631944444444444</v>
       </c>
-      <c r="D3" s="100">
+      <c r="E3" s="99">
         <v>47.2</v>
       </c>
-      <c r="E3" s="100">
+      <c r="F3" s="102">
         <v>96.5</v>
       </c>
+      <c r="G3" s="99">
+        <v>6.0</v>
+      </c>
+      <c r="H3" s="99">
+        <v>22.8</v>
+      </c>
+      <c r="I3" s="99" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" s="99" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="102">
+      <c r="A4" s="99" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="100">
         <v>45262.0</v>
       </c>
-      <c r="B4" s="100" t="s">
+      <c r="C4" s="104" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="101">
+      <c r="D4" s="101">
         <v>0.6354166666666666</v>
       </c>
-      <c r="D4" s="100">
+      <c r="E4" s="99">
         <v>47.2</v>
       </c>
-      <c r="E4" s="100">
+      <c r="F4" s="102">
         <v>96.5</v>
       </c>
+      <c r="G4" s="99">
+        <v>8.0</v>
+      </c>
+      <c r="H4" s="99">
+        <v>20.8</v>
+      </c>
+      <c r="I4" s="99" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="99" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="102">
+      <c r="A5" s="99" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="100">
         <v>45262.0</v>
       </c>
-      <c r="B5" s="100" t="s">
+      <c r="C5" s="104" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="101">
+      <c r="D5" s="101">
         <v>0.6930555555555555</v>
       </c>
-      <c r="D5" s="100">
+      <c r="E5" s="114">
         <v>173.0</v>
       </c>
-      <c r="E5" s="100">
+      <c r="F5" s="114">
         <v>167.0</v>
       </c>
+      <c r="G5" s="114">
+        <v>2.3</v>
+      </c>
+      <c r="H5" s="114">
+        <v>1.28</v>
+      </c>
+      <c r="I5" s="99" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="99" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="102">
+      <c r="A6" s="103" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="113">
         <v>45264.0</v>
       </c>
-      <c r="B6" s="100" t="s">
+      <c r="C6" s="103" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="101">
+      <c r="D6" s="109">
         <v>0.4340277777777778</v>
       </c>
-      <c r="D6" s="100">
+      <c r="E6" s="103">
         <v>0.45</v>
       </c>
-      <c r="E6" s="100">
+      <c r="F6" s="110">
         <v>3.88</v>
       </c>
+      <c r="G6" s="103">
+        <v>14.8</v>
+      </c>
+      <c r="H6" s="103">
+        <v>94.5</v>
+      </c>
+      <c r="I6" s="103" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="103" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="102">
+      <c r="A7" s="99" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="100">
         <v>45264.0</v>
       </c>
-      <c r="B7" s="100" t="s">
+      <c r="C7" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="101">
+      <c r="D7" s="101">
         <v>0.5708333333333333</v>
       </c>
-      <c r="D7" s="100">
+      <c r="E7" s="99">
         <v>2.63</v>
       </c>
-      <c r="E7" s="100">
+      <c r="F7" s="102">
         <v>9.13</v>
       </c>
+      <c r="G7" s="99">
+        <v>21.5</v>
+      </c>
+      <c r="H7" s="99">
+        <v>1109.0</v>
+      </c>
+      <c r="I7" s="99" t="s">
+        <v>39</v>
+      </c>
+      <c r="J7" s="99" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="102">
+      <c r="A8" s="99" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="100">
         <v>45264.0</v>
       </c>
-      <c r="B8" s="100" t="s">
+      <c r="C8" s="104" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="101">
+      <c r="D8" s="101">
         <v>0.1284722222222222</v>
       </c>
-      <c r="D8" s="100">
+      <c r="E8" s="99">
         <v>0.57</v>
       </c>
-      <c r="E8" s="100">
+      <c r="F8" s="102">
         <v>6.85</v>
       </c>
+      <c r="G8" s="99">
+        <v>498.0</v>
+      </c>
+      <c r="H8" s="99">
+        <v>536.0</v>
+      </c>
+      <c r="I8" s="99" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="99" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="102">
+      <c r="A9" s="99" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="100">
         <v>45264.0</v>
       </c>
-      <c r="B9" s="100" t="s">
+      <c r="C9" s="104" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="101">
+      <c r="D9" s="101">
         <v>0.6909722222222222</v>
       </c>
-      <c r="D9" s="100">
+      <c r="E9" s="114">
         <v>186.0</v>
       </c>
-      <c r="E9" s="100">
+      <c r="F9" s="114">
         <v>58.1</v>
       </c>
+      <c r="G9" s="114">
+        <v>4.2</v>
+      </c>
+      <c r="H9" s="114">
+        <v>98.0</v>
+      </c>
+      <c r="I9" s="99" t="s">
+        <v>39</v>
+      </c>
+      <c r="J9" s="99" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="102">
+      <c r="A10" s="103" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="113">
         <v>45265.0</v>
       </c>
-      <c r="B10" s="100" t="s">
+      <c r="C10" s="103" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="101">
+      <c r="D10" s="109">
         <v>0.4340277777777778</v>
       </c>
-      <c r="D10" s="100">
+      <c r="E10" s="103">
         <v>8.71</v>
       </c>
-      <c r="E10" s="100">
+      <c r="F10" s="110">
         <v>64.3</v>
       </c>
+      <c r="G10" s="103">
+        <v>7.0</v>
+      </c>
+      <c r="H10" s="103">
+        <v>25.6</v>
+      </c>
+      <c r="I10" s="99" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10" s="99" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="102">
+      <c r="A11" s="99" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="100">
         <v>45265.0</v>
       </c>
-      <c r="B11" s="100" t="s">
+      <c r="C11" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="101">
+      <c r="D11" s="101">
         <v>0.5611111111111111</v>
       </c>
-      <c r="D11" s="100">
+      <c r="E11" s="99">
         <v>8.66</v>
       </c>
-      <c r="E11" s="100">
+      <c r="F11" s="102">
         <v>16.1</v>
       </c>
+      <c r="G11" s="99">
+        <v>63.0</v>
+      </c>
+      <c r="H11" s="99">
+        <v>101.0</v>
+      </c>
+      <c r="I11" s="99" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11" s="99" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="102">
+      <c r="A12" s="99" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="100">
         <v>45265.0</v>
       </c>
-      <c r="B12" s="100" t="s">
+      <c r="C12" s="104" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="101">
+      <c r="D12" s="101">
         <v>0.6423611111111112</v>
       </c>
-      <c r="D12" s="100">
+      <c r="E12" s="99">
         <v>0.48</v>
       </c>
-      <c r="E12" s="100">
+      <c r="F12" s="102">
         <v>11.0</v>
       </c>
+      <c r="G12" s="99">
+        <v>14.0</v>
+      </c>
+      <c r="H12" s="99">
+        <v>98.7</v>
+      </c>
+      <c r="I12" s="99" t="s">
+        <v>39</v>
+      </c>
+      <c r="J12" s="99" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="102">
+      <c r="A13" s="99" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="100">
         <v>45265.0</v>
       </c>
-      <c r="B13" s="100" t="s">
+      <c r="C13" s="104" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="101">
+      <c r="D13" s="101">
         <v>0.6881944444444444</v>
       </c>
-      <c r="D13" s="100">
+      <c r="E13" s="99">
         <v>153.0</v>
       </c>
-      <c r="E13" s="100">
+      <c r="F13" s="102">
         <v>178.0</v>
       </c>
+      <c r="G13" s="99">
+        <v>3.0</v>
+      </c>
+      <c r="H13" s="99">
+        <v>0.53</v>
+      </c>
+      <c r="I13" s="99" t="s">
+        <v>39</v>
+      </c>
+      <c r="J13" s="99" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="102">
+      <c r="A14" s="103" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="113">
         <v>45266.0</v>
       </c>
-      <c r="B14" s="100" t="s">
+      <c r="C14" s="103" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="103">
+      <c r="D14" s="115">
         <v>0.42986111111111114</v>
       </c>
-      <c r="D14" s="100">
+      <c r="E14" s="114">
         <v>9.53</v>
       </c>
-      <c r="E14" s="100">
+      <c r="F14" s="114">
         <v>11.4</v>
       </c>
+      <c r="G14" s="114">
+        <v>14.5</v>
+      </c>
+      <c r="H14" s="114">
+        <v>30.8</v>
+      </c>
+      <c r="I14" s="103" t="s">
+        <v>70</v>
+      </c>
+      <c r="J14" s="116"/>
     </row>
     <row r="15">
-      <c r="A15" s="102">
+      <c r="A15" s="99" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="100">
         <v>45266.0</v>
       </c>
-      <c r="B15" s="100" t="s">
+      <c r="C15" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="101">
+      <c r="D15" s="101">
         <v>0.5618055555555556</v>
       </c>
-      <c r="D15" s="100">
+      <c r="E15" s="99">
         <v>6.9</v>
       </c>
-      <c r="E15" s="100">
+      <c r="F15" s="102">
         <v>21.1</v>
+      </c>
+      <c r="G15" s="99">
+        <v>5.0</v>
+      </c>
+      <c r="H15" s="99">
+        <v>27.4</v>
+      </c>
+      <c r="I15" s="108"/>
+      <c r="J15" s="108"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="99" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="100">
+        <v>45266.0</v>
+      </c>
+      <c r="C16" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="117">
+        <v>0.6354166666666666</v>
+      </c>
+      <c r="E16" s="114">
+        <v>2.38</v>
+      </c>
+      <c r="F16" s="114">
+        <v>10.6</v>
+      </c>
+      <c r="G16" s="114">
+        <v>16.0</v>
+      </c>
+      <c r="H16" s="114">
+        <v>412.0</v>
+      </c>
+      <c r="J16" s="108"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="99" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="100">
+        <v>45266.0</v>
+      </c>
+      <c r="C17" s="104" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="101">
+        <v>0.6881944444444444</v>
+      </c>
+      <c r="E17" s="99">
+        <v>2.93</v>
+      </c>
+      <c r="F17" s="102">
+        <v>13.4</v>
+      </c>
+      <c r="G17" s="99">
+        <v>4.0</v>
+      </c>
+      <c r="H17" s="99">
+        <v>20.6</v>
+      </c>
+      <c r="I17" s="108"/>
+      <c r="J17" s="108"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:J17">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
+      <formula>LEN(TRIM(A1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <drawing r:id="rId1"/>
+  <tableParts count="4">
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="17.88"/>
+    <col customWidth="1" min="3" max="3" width="15.75"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="114" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="114" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="114" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="118">
+        <v>45262.0</v>
+      </c>
+      <c r="B2" s="119">
+        <f>Hanson!E2-'Old Main'!E2</f>
+        <v>-72</v>
+      </c>
+      <c r="C2" s="119">
+        <f>Hanson!F2-'Old Main'!F2</f>
+        <v>-157</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="118">
+        <v>45262.0</v>
+      </c>
+      <c r="B3" s="119">
+        <f>Hanson!E3-'Old Main'!E3</f>
+        <v>50.6</v>
+      </c>
+      <c r="C3" s="119">
+        <f>Hanson!F3-'Old Main'!F3</f>
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="118">
+        <v>45262.0</v>
+      </c>
+      <c r="B4" s="119">
+        <f>Hanson!E4-'Old Main'!E4</f>
+        <v>50.1</v>
+      </c>
+      <c r="C4" s="119">
+        <f>Hanson!F4-'Old Main'!F4</f>
+        <v>-6.2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="118">
+        <v>45262.0</v>
+      </c>
+      <c r="B5" s="119">
+        <f>Hanson!E5-'Old Main'!E5</f>
+        <v>-128.1</v>
+      </c>
+      <c r="C5" s="119">
+        <f>Hanson!F5-'Old Main'!F5</f>
+        <v>-79</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="118">
+        <v>45264.0</v>
+      </c>
+      <c r="B6" s="119">
+        <f>Hanson!E6-'Old Main'!E6</f>
+        <v>27.75</v>
+      </c>
+      <c r="C6" s="119">
+        <f>Hanson!F6-'Old Main'!F6</f>
+        <v>58.82</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="118">
+        <v>45264.0</v>
+      </c>
+      <c r="B7" s="119">
+        <f>Hanson!E7-'Old Main'!E7</f>
+        <v>33.17</v>
+      </c>
+      <c r="C7" s="119">
+        <f>Hanson!F7-'Old Main'!F7</f>
+        <v>17.97</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="118">
+        <v>45264.0</v>
+      </c>
+      <c r="B8" s="119">
+        <f>Hanson!E8-'Old Main'!E8</f>
+        <v>67.93</v>
+      </c>
+      <c r="C8" s="119">
+        <f>Hanson!F8-'Old Main'!F8</f>
+        <v>19.75</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="118">
+        <v>45264.0</v>
+      </c>
+      <c r="B9" s="119">
+        <f>Hanson!E9-'Old Main'!E9</f>
+        <v>-62</v>
+      </c>
+      <c r="C9" s="119">
+        <f>Hanson!F9-'Old Main'!F9</f>
+        <v>-1.4</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="118">
+        <v>45265.0</v>
+      </c>
+      <c r="B10" s="119">
+        <f>Hanson!E10-'Old Main'!E10</f>
+        <v>-7.37</v>
+      </c>
+      <c r="C10" s="119">
+        <f>Hanson!F10-'Old Main'!F10</f>
+        <v>-62.61</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="118">
+        <v>45265.0</v>
+      </c>
+      <c r="B11" s="119">
+        <f>Hanson!E11-'Old Main'!E11</f>
+        <v>2.64</v>
+      </c>
+      <c r="C11" s="119">
+        <f>Hanson!F11-'Old Main'!F11</f>
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="118">
+        <v>45265.0</v>
+      </c>
+      <c r="B12" s="119">
+        <f>Hanson!E12-'Old Main'!E12</f>
+        <v>139.52</v>
+      </c>
+      <c r="C12" s="119">
+        <f>Hanson!F12-'Old Main'!F12</f>
+        <v>70.4</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="118">
+        <v>45265.0</v>
+      </c>
+      <c r="B13" s="119">
+        <f>Hanson!E13-'Old Main'!E13</f>
+        <v>92</v>
+      </c>
+      <c r="C13" s="119">
+        <f>Hanson!F13-'Old Main'!F13</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="118">
+        <v>45266.0</v>
+      </c>
+      <c r="B14" s="119">
+        <f>Hanson!E14-'Old Main'!E14</f>
+        <v>-4.91</v>
+      </c>
+      <c r="C14" s="119">
+        <f>Hanson!F14-'Old Main'!F14</f>
+        <v>25.9</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="118">
+        <v>45266.0</v>
+      </c>
+      <c r="B15" s="119">
+        <f>Hanson!E15-'Old Main'!E15</f>
+        <v>54.9</v>
+      </c>
+      <c r="C15" s="119">
+        <f>Hanson!F15-'Old Main'!F15</f>
+        <v>83.9</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="118">
+        <v>45266.0</v>
+      </c>
+      <c r="B16" s="119">
+        <f>Hanson!E16-'Old Main'!E16</f>
+        <v>103.62</v>
+      </c>
+      <c r="C16" s="119">
+        <f>Hanson!F16-'Old Main'!F16</f>
+        <v>128.4</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="118">
+        <v>45266.0</v>
+      </c>
+      <c r="B17" s="119">
+        <f>Hanson!E17-'Old Main'!E17</f>
+        <v>17.47</v>
+      </c>
+      <c r="C17" s="119">
+        <f>Hanson!F17-'Old Main'!F17</f>
+        <v>36.8</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="114" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="119">
+        <f t="shared" ref="B18:C18" si="1">AVERAGE(B2:B17)</f>
+        <v>22.8325</v>
+      </c>
+      <c r="C18" s="119">
+        <f t="shared" si="1"/>
+        <v>9.639375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>